<commit_message>
Added local BSol shape files
</commit_message>
<xml_diff>
--- a/brum_ward_info.xlsx
+++ b/brum_ward_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SVWCCG111\publichealth$\2.0 KNOWLEDGE EVIDENCE &amp; GOVERNANCE - KEG\2.8 GIS RESOURCES\GP-mapping-tool\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/MiscCode/GP-mapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC56B138-3970-486D-B53D-EFA5FFC2A9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CC56B138-3970-486D-B53D-EFA5FFC2A9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{493FF97E-199F-4012-9908-3E4877EB690F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -1625,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7324DB63-4271-4AE6-9379-21339453ADFC}">
   <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1650,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>

</xml_diff>